<commit_message>
some ppt is big, and to delete many pictures.
</commit_message>
<xml_diff>
--- a/2017 PPES Lookout Project--001/005. Training Methods/2017PPES【005.TM】.xlsx
+++ b/2017 PPES Lookout Project--001/005. Training Methods/2017PPES【005.TM】.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\【003 THESIS】論述.201508-\2018博士論文\20180111 Github實作2017PPES\2017 PPES Lookout Project--001\005. Training Methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\【003 THESIS】論述.201508-\2018博士論文\20180111 Github實作2017PPES\2017 PPES on Github\2017 PPES Lookout Project--001\005. Training Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -778,7 +778,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>

</xml_diff>